<commit_message>
improve scholars summary export to filter based on scholarship type
</commit_message>
<xml_diff>
--- a/storage/templates/scholars profile summary.xlsx
+++ b/storage/templates/scholars profile summary.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="24045" windowHeight="12480"/>
+    <workbookView windowWidth="27945" windowHeight="12480"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -108,7 +108,7 @@
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="178" formatCode="00000000000"/>
   </numFmts>
-  <fonts count="33">
+  <fonts count="32">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -201,13 +201,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -352,7 +345,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="36">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -548,12 +541,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -576,21 +563,6 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
       <bottom style="thin">
         <color auto="1"/>
       </bottom>
@@ -622,6 +594,34 @@
     </border>
     <border>
       <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right/>
       <top style="thin">
         <color auto="1"/>
@@ -634,19 +634,6 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
         <color auto="1"/>
       </bottom>
       <diagonal/>
@@ -752,152 +739,152 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="176" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="6" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="7" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="7" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="8" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="7" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="7" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="8" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -909,25 +896,34 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -936,22 +932,22 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="3" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="3" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="178" fontId="5" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="5" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="3" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="3" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -977,14 +973,14 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1356,7 +1352,7 @@
   <dimension ref="A1:N25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="63" zoomScaleNormal="63" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="A6" sqref="A6:C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -1456,10 +1452,10 @@
       <c r="M5" s="3"/>
       <c r="N5" s="3"/>
     </row>
-    <row r="6" spans="1:14">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
+    <row r="6" ht="35" customHeight="1" spans="1:14">
+      <c r="A6" s="4"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="6"/>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
@@ -1473,197 +1469,198 @@
       <c r="N6" s="3"/>
     </row>
     <row r="7" ht="33" spans="1:14">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E7" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F7" s="5" t="s">
+      <c r="F7" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="G7" s="5" t="s">
+      <c r="G7" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="H7" s="4" t="s">
+      <c r="H7" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="I7" s="4" t="s">
+      <c r="I7" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="J7" s="4" t="s">
+      <c r="J7" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="K7" s="4" t="s">
+      <c r="K7" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="L7" s="4" t="s">
+      <c r="L7" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="M7" s="4" t="s">
+      <c r="M7" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="N7" s="4" t="s">
+      <c r="N7" s="7" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:14">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
-      <c r="J8" s="7"/>
-      <c r="K8" s="7"/>
-      <c r="L8" s="7"/>
-      <c r="M8" s="7"/>
-      <c r="N8" s="34"/>
+      <c r="B8" s="10"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="10"/>
+      <c r="K8" s="10"/>
+      <c r="L8" s="10"/>
+      <c r="M8" s="10"/>
+      <c r="N8" s="37"/>
     </row>
     <row r="9" spans="1:14">
-      <c r="A9" s="9"/>
-      <c r="B9" s="9"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
-      <c r="H9" s="9"/>
-      <c r="I9" s="9"/>
-      <c r="J9" s="9"/>
-      <c r="K9" s="9"/>
-      <c r="L9" s="9"/>
-      <c r="M9" s="9"/>
-      <c r="N9" s="9"/>
+      <c r="A9" s="12"/>
+      <c r="B9" s="12"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="12"/>
+      <c r="I9" s="12"/>
+      <c r="J9" s="12"/>
+      <c r="K9" s="12"/>
+      <c r="L9" s="12"/>
+      <c r="M9" s="12"/>
+      <c r="N9" s="12"/>
     </row>
     <row r="10" spans="1:14">
-      <c r="A10" s="10" t="s">
+      <c r="A10" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="10"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="10"/>
-      <c r="H10" s="10"/>
-      <c r="I10" s="10"/>
-      <c r="J10" s="10"/>
-      <c r="K10" s="10"/>
-      <c r="L10" s="10"/>
-      <c r="M10" s="10"/>
-      <c r="N10" s="10"/>
+      <c r="B10" s="13"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="13"/>
+      <c r="I10" s="13"/>
+      <c r="J10" s="13"/>
+      <c r="K10" s="13"/>
+      <c r="L10" s="13"/>
+      <c r="M10" s="13"/>
+      <c r="N10" s="13"/>
     </row>
     <row r="11" spans="1:14">
-      <c r="A11" s="9"/>
-      <c r="B11" s="9"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9"/>
-      <c r="H11" s="9"/>
-      <c r="I11" s="9"/>
-      <c r="J11" s="9"/>
-      <c r="K11" s="9"/>
-      <c r="L11" s="9"/>
-      <c r="M11" s="9"/>
-      <c r="N11" s="9"/>
+      <c r="A11" s="12"/>
+      <c r="B11" s="12"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="12"/>
+      <c r="I11" s="12"/>
+      <c r="J11" s="12"/>
+      <c r="K11" s="12"/>
+      <c r="L11" s="12"/>
+      <c r="M11" s="12"/>
+      <c r="N11" s="12"/>
     </row>
     <row r="12" ht="20.75" customHeight="1"/>
     <row r="13" ht="15.65" customHeight="1" spans="2:4">
-      <c r="B13" s="11" t="s">
+      <c r="B13" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="12"/>
-      <c r="D13" s="13"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="16"/>
     </row>
     <row r="14" ht="15.75" spans="2:3">
-      <c r="B14" s="14" t="s">
+      <c r="B14" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="C14" s="15"/>
+      <c r="C14" s="18"/>
     </row>
     <row r="15" ht="15.75" spans="2:3">
-      <c r="B15" s="16" t="s">
+      <c r="B15" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="C15" s="17"/>
+      <c r="C15" s="20"/>
     </row>
     <row r="16" ht="15.75" spans="2:3">
-      <c r="B16" s="18" t="s">
+      <c r="B16" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="C16" s="19"/>
+      <c r="C16" s="22"/>
     </row>
     <row r="19" spans="4:8">
-      <c r="D19" s="20" t="s">
+      <c r="D19" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="E19" s="21"/>
-      <c r="G19" s="22" t="s">
+      <c r="E19" s="24"/>
+      <c r="G19" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="H19" s="23"/>
+      <c r="H19" s="26"/>
     </row>
     <row r="20" spans="4:8">
-      <c r="D20" s="24"/>
-      <c r="E20" s="25" t="s">
+      <c r="D20" s="27"/>
+      <c r="E20" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="G20" s="26"/>
-      <c r="H20" s="25" t="s">
+      <c r="G20" s="29"/>
+      <c r="H20" s="28" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="21" spans="4:8">
-      <c r="D21" s="24"/>
-      <c r="E21" s="27" t="s">
+      <c r="D21" s="27"/>
+      <c r="E21" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="G21" s="26"/>
-      <c r="H21" s="27" t="s">
+      <c r="G21" s="29"/>
+      <c r="H21" s="30" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="22" ht="15.75" spans="4:5">
-      <c r="D22" s="28"/>
-      <c r="E22" s="29"/>
+      <c r="D22" s="31"/>
+      <c r="E22" s="32"/>
     </row>
     <row r="23" ht="15.75" spans="4:5">
-      <c r="D23" s="28"/>
-      <c r="E23" s="30"/>
+      <c r="D23" s="31"/>
+      <c r="E23" s="33"/>
     </row>
     <row r="24" ht="16.5" spans="4:8">
-      <c r="D24" s="28"/>
-      <c r="E24" s="31"/>
-      <c r="H24" s="32"/>
+      <c r="D24" s="31"/>
+      <c r="E24" s="34"/>
+      <c r="H24" s="35"/>
     </row>
     <row r="25" ht="15.75" spans="4:8">
-      <c r="D25" s="28"/>
-      <c r="E25" s="33" t="s">
+      <c r="D25" s="31"/>
+      <c r="E25" s="36" t="s">
         <v>26</v>
       </c>
-      <c r="H25" s="33" t="s">
+      <c r="H25" s="36" t="s">
         <v>26</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
+    <mergeCell ref="A6:C6"/>
     <mergeCell ref="A8:N8"/>
     <mergeCell ref="A10:N10"/>
     <mergeCell ref="A1:N3"/>

</xml_diff>